<commit_message>
Update source excel file.
</commit_message>
<xml_diff>
--- a/sample/sample.xlsx
+++ b/sample/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharry.xu\source\repos\jira-tool\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sharry.xu\source\repos\jira-tool\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864EF82E-2B32-409A-AC37-9CC60C36DE44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D7898E-0B00-4F74-8E37-6B0515CF56D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" firstSheet="2" activeTab="2" xr2:uid="{CDBCB60A-DAE4-4524-ABE8-B57A913684F2}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3296" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3347" uniqueCount="623">
   <si>
     <t>Combined Release Schedule (Legacy &amp; BUX)</t>
   </si>
@@ -1925,6 +1925,33 @@
   </si>
   <si>
     <t>June 13,2023</t>
+  </si>
+  <si>
+    <t>John Rease</t>
+  </si>
+  <si>
+    <t>Harold Finch</t>
+  </si>
+  <si>
+    <t>Tony Wei</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>PO Review</t>
+  </si>
+  <si>
+    <t>Sign Off</t>
+  </si>
+  <si>
+    <t>https://jira.com/browse/proj-003</t>
+  </si>
+  <si>
+    <t>https://jira.com/browse/proj-004</t>
+  </si>
+  <si>
+    <t>https://jira.com/browse/proj-005</t>
   </si>
 </sst>
 </file>
@@ -2992,22 +3019,25 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="12" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3036,9 +3066,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3374,10 +3401,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="9" customFormat="1" ht="78.650000000000006" customHeight="1">
-      <c r="A1" s="141" t="s">
+      <c r="A1" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="142"/>
+      <c r="B1" s="143"/>
     </row>
     <row r="2" spans="1:2" s="10" customFormat="1" ht="31">
       <c r="A2" s="12" t="s">
@@ -3614,32 +3641,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.5" thickBot="1">
-      <c r="A1" s="147" t="s">
+      <c r="A1" s="148" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
-      <c r="D1" s="149"/>
+      <c r="B1" s="149"/>
+      <c r="C1" s="149"/>
+      <c r="D1" s="150"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="150" t="s">
+      <c r="A2" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="153" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="152" t="s">
+      <c r="C2" s="153" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="154" t="s">
+      <c r="D2" s="155" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1">
-      <c r="A3" s="151"/>
-      <c r="B3" s="153"/>
-      <c r="C3" s="153"/>
-      <c r="D3" s="155"/>
+      <c r="A3" s="152"/>
+      <c r="B3" s="154"/>
+      <c r="C3" s="154"/>
+      <c r="D3" s="156"/>
     </row>
     <row r="4" spans="1:4" ht="46.5">
       <c r="A4" s="34" t="s">
@@ -3656,10 +3683,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="31">
-      <c r="A5" s="144" t="s">
+      <c r="A5" s="146" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="143" t="s">
+      <c r="B5" s="147" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -3670,8 +3697,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="31">
-      <c r="A6" s="144"/>
-      <c r="B6" s="143"/>
+      <c r="A6" s="146"/>
+      <c r="B6" s="147"/>
       <c r="C6" s="14" t="s">
         <v>40</v>
       </c>
@@ -3680,10 +3707,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="31">
-      <c r="A7" s="144" t="s">
+      <c r="A7" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="143" t="s">
+      <c r="B7" s="147" t="s">
         <v>43</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -3694,8 +3721,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="31">
-      <c r="A8" s="144"/>
-      <c r="B8" s="143"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="147"/>
       <c r="C8" s="14" t="s">
         <v>46</v>
       </c>
@@ -3704,8 +3731,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.5">
-      <c r="A9" s="144"/>
-      <c r="B9" s="143"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="147"/>
       <c r="C9" s="14" t="s">
         <v>48</v>
       </c>
@@ -3714,8 +3741,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="31">
-      <c r="A10" s="144"/>
-      <c r="B10" s="143"/>
+      <c r="A10" s="146"/>
+      <c r="B10" s="147"/>
       <c r="C10" s="14" t="s">
         <v>50</v>
       </c>
@@ -3724,10 +3751,10 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="31">
-      <c r="A11" s="144" t="s">
+      <c r="A11" s="146" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="143" t="s">
+      <c r="B11" s="147" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -3738,8 +3765,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="46.5">
-      <c r="A12" s="144"/>
-      <c r="B12" s="143"/>
+      <c r="A12" s="146"/>
+      <c r="B12" s="147"/>
       <c r="C12" s="14" t="s">
         <v>48</v>
       </c>
@@ -3748,8 +3775,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.5">
-      <c r="A13" s="144"/>
-      <c r="B13" s="143"/>
+      <c r="A13" s="146"/>
+      <c r="B13" s="147"/>
       <c r="C13" s="14" t="s">
         <v>50</v>
       </c>
@@ -3758,10 +3785,10 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="31">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="146" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="143" t="s">
+      <c r="B14" s="147" t="s">
         <v>58</v>
       </c>
       <c r="C14" s="14" t="s">
@@ -3772,8 +3799,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="46.5">
-      <c r="A15" s="144"/>
-      <c r="B15" s="143"/>
+      <c r="A15" s="146"/>
+      <c r="B15" s="147"/>
       <c r="C15" s="14" t="s">
         <v>48</v>
       </c>
@@ -3782,8 +3809,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.5">
-      <c r="A16" s="144"/>
-      <c r="B16" s="143"/>
+      <c r="A16" s="146"/>
+      <c r="B16" s="147"/>
       <c r="C16" s="14" t="s">
         <v>50</v>
       </c>
@@ -3792,10 +3819,10 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="31">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="146" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="143" t="s">
+      <c r="B17" s="147" t="s">
         <v>61</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -3806,8 +3833,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.5">
-      <c r="A18" s="144"/>
-      <c r="B18" s="143"/>
+      <c r="A18" s="146"/>
+      <c r="B18" s="147"/>
       <c r="C18" s="14" t="s">
         <v>48</v>
       </c>
@@ -3816,8 +3843,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.5">
-      <c r="A19" s="144"/>
-      <c r="B19" s="143"/>
+      <c r="A19" s="146"/>
+      <c r="B19" s="147"/>
       <c r="C19" s="14" t="s">
         <v>50</v>
       </c>
@@ -3826,10 +3853,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.5">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="146" t="s">
         <v>65</v>
       </c>
-      <c r="B20" s="143" t="s">
+      <c r="B20" s="147" t="s">
         <v>66</v>
       </c>
       <c r="C20" s="14" t="s">
@@ -3840,8 +3867,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.5">
-      <c r="A21" s="144"/>
-      <c r="B21" s="143"/>
+      <c r="A21" s="146"/>
+      <c r="B21" s="147"/>
       <c r="C21" s="14" t="s">
         <v>46</v>
       </c>
@@ -3850,8 +3877,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.5">
-      <c r="A22" s="144"/>
-      <c r="B22" s="143"/>
+      <c r="A22" s="146"/>
+      <c r="B22" s="147"/>
       <c r="C22" s="14" t="s">
         <v>48</v>
       </c>
@@ -3860,8 +3887,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.5">
-      <c r="A23" s="144"/>
-      <c r="B23" s="143"/>
+      <c r="A23" s="146"/>
+      <c r="B23" s="147"/>
       <c r="C23" s="14" t="s">
         <v>50</v>
       </c>
@@ -3870,10 +3897,10 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.5">
-      <c r="A24" s="144" t="s">
+      <c r="A24" s="146" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="143" t="s">
+      <c r="B24" s="147" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -3884,8 +3911,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="31">
-      <c r="A25" s="144"/>
-      <c r="B25" s="143"/>
+      <c r="A25" s="146"/>
+      <c r="B25" s="147"/>
       <c r="C25" s="14" t="s">
         <v>48</v>
       </c>
@@ -3894,8 +3921,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="31">
-      <c r="A26" s="144"/>
-      <c r="B26" s="143"/>
+      <c r="A26" s="146"/>
+      <c r="B26" s="147"/>
       <c r="C26" s="14" t="s">
         <v>50</v>
       </c>
@@ -3918,10 +3945,10 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="31">
-      <c r="A28" s="145" t="s">
+      <c r="A28" s="144" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="146" t="s">
+      <c r="B28" s="145" t="s">
         <v>81</v>
       </c>
       <c r="C28" s="33" t="s">
@@ -3932,8 +3959,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="31">
-      <c r="A29" s="145"/>
-      <c r="B29" s="146"/>
+      <c r="A29" s="144"/>
+      <c r="B29" s="145"/>
       <c r="C29" s="33" t="s">
         <v>48</v>
       </c>
@@ -3942,8 +3969,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="31">
-      <c r="A30" s="145"/>
-      <c r="B30" s="146"/>
+      <c r="A30" s="144"/>
+      <c r="B30" s="145"/>
       <c r="C30" s="33" t="s">
         <v>50</v>
       </c>
@@ -3959,6 +3986,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
     <mergeCell ref="A28:A30"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="A5:A6"/>
@@ -3975,11 +4007,6 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3991,7 +4018,7 @@
   <dimension ref="A1:R1048364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4080,7 +4107,7 @@
       <c r="C2" s="135" t="s">
         <v>608</v>
       </c>
-      <c r="D2" s="156" t="s">
+      <c r="D2" s="141" t="s">
         <v>610</v>
       </c>
       <c r="E2" s="48" t="s">
@@ -4146,7 +4173,7 @@
         <v>110</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>44</v>
+        <v>105</v>
       </c>
       <c r="H3" s="49" t="s">
         <v>104</v>
@@ -4183,55 +4210,172 @@
       </c>
     </row>
     <row r="4" spans="1:18">
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
+      <c r="A4" s="66" t="s">
+        <v>613</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>614</v>
+      </c>
+      <c r="C4" s="135" t="s">
+        <v>617</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>620</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="L4" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="O4" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="P4" s="140">
+        <v>44706</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="5" spans="1:18">
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
+      <c r="A5" s="66" t="s">
+        <v>613</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>615</v>
+      </c>
+      <c r="C5" s="135" t="s">
+        <v>618</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>621</v>
+      </c>
+      <c r="E5" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="L5" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="N5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="O5" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="P5" s="140">
+        <v>44706</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="6" spans="1:18">
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
+      <c r="A6" s="66" t="s">
+        <v>613</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>616</v>
+      </c>
+      <c r="C6" s="135" t="s">
+        <v>619</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>622</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="O6" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="P6" s="140">
+        <v>44706</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:18">
       <c r="D7" s="8"/>
@@ -4801,9 +4945,12 @@
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{D43640AC-0365-4F94-A12D-172584DA6CD3}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{CC70641A-AC8E-4033-80E8-BC07D5E8E0A1}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{AEA56A19-EBF9-4936-84AD-09C046A47142}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{E997C9DD-7E86-4100-944F-4716EF0454EC}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{05DBA1DB-899B-48E3-9842-1706FF8C8E78}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
@@ -4811,19 +4958,19 @@
           <x14:formula1>
             <xm:f>Data!$C$3:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M3 N1:N3 M4:N1048576 H2:J1048576</xm:sqref>
+          <xm:sqref>M2:M6 N1:N6 H2:J1048576 M7:N1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A449802B-31AE-4A29-9E5C-3EF9960FB2C6}">
           <x14:formula1>
             <xm:f>Data!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O1:O1048576 F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F1048576 O1:O1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{94063A04-C517-4097-ADF2-A164B4C763A6}">
           <x14:formula1>
             <xm:f>Data!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576 G2:G1048576</xm:sqref>
+          <xm:sqref>G2:G1048576 L2:L1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0CDDDF5C-0F2A-4E47-850E-981C560DB5F4}">
           <x14:formula1>

</xml_diff>